<commit_message>
Updated test results (MAGNAN)
Some earlier data were not checked in! (VaxiJen)
</commit_message>
<xml_diff>
--- a/Code/R/Data.xlsx
+++ b/Code/R/Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Profile</t>
   </si>
@@ -114,6 +114,27 @@
   </si>
   <si>
     <t>nGDip</t>
+  </si>
+  <si>
+    <t>out_1152_nGDip</t>
+  </si>
+  <si>
+    <t>out_1152_ngrams</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>out_1152_PSF</t>
+  </si>
+  <si>
+    <t>Magnan</t>
+  </si>
+  <si>
+    <t>VaxiJen</t>
   </si>
 </sst>
 </file>
@@ -762,21 +783,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
+    <row r="1" spans="1:11" ht="30">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -793,100 +814,186 @@
         <v>23</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="2"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="2">
+        <v>800</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.01</v>
+      </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2"/>
+      <c r="F2" s="6">
+        <v>0.78366130000000001</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.72222220000000004</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0.67708330000000005</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0.76736110000000002</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0.44626670000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="2"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="C4" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4">
+        <v>0.68897388599536902</v>
+      </c>
+      <c r="G4">
+        <v>0.66927083333333304</v>
+      </c>
+      <c r="H4">
+        <v>0.57118055555555602</v>
+      </c>
+      <c r="I4">
+        <v>0.76736111111111105</v>
+      </c>
+      <c r="J4">
+        <v>0.34525065000504301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="F6" s="2"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17">
+        <v>0.81</v>
+      </c>
+      <c r="G17">
+        <v>0.75509999999999999</v>
+      </c>
+      <c r="H17">
+        <v>0.75880000000000003</v>
+      </c>
+      <c r="I17">
+        <v>0.75139999999999996</v>
+      </c>
+      <c r="J17">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18">
+        <v>0.67</v>
+      </c>
+      <c r="G18">
+        <v>0.5948</v>
+      </c>
+      <c r="H18">
+        <v>0.89690000000000003</v>
+      </c>
+      <c r="I18">
+        <v>0.25850000000000001</v>
+      </c>
+      <c r="J18">
+        <v>0.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Moved sequences to another subfolder.
Updates.
</commit_message>
<xml_diff>
--- a/Code/R/Data.xlsx
+++ b/Code/R/Data.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Vaxi" sheetId="1" r:id="rId1"/>
     <sheet name="Magnan_10FoldCV" sheetId="3" r:id="rId2"/>
+    <sheet name="IndependentTests" sheetId="4" r:id="rId3"/>
+    <sheet name="Enrichment" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>Profile</t>
   </si>
@@ -135,6 +137,42 @@
   </si>
   <si>
     <t>VaxiJen</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>MAGNAN</t>
+  </si>
+  <si>
+    <t>out_1152_nGrams</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>ANTIGENpro</t>
+  </si>
+  <si>
+    <t>SignalP</t>
+  </si>
+  <si>
+    <t>Vaxijen</t>
+  </si>
+  <si>
+    <t>Top ranked 2%</t>
+  </si>
+  <si>
+    <t>Top ranked 5%</t>
+  </si>
+  <si>
+    <t>Top ranked 10%</t>
+  </si>
+  <si>
+    <t>Top ranked 25%</t>
   </si>
 </sst>
 </file>
@@ -187,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -203,6 +241,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -867,13 +918,30 @@
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="C3" s="2">
+        <v>1100</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.8290805</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.75607639999999998</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.77951389999999998</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.73263889999999998</v>
+      </c>
+      <c r="J3">
+        <v>0.51271639999999996</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
@@ -941,7 +1009,7 @@
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="2"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -996,4 +1064,430 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="7"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E3">
+        <v>0.6</v>
+      </c>
+      <c r="F3">
+        <v>0.65</v>
+      </c>
+      <c r="G3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="8"/>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>61.64</v>
+      </c>
+      <c r="D4">
+        <v>57.53</v>
+      </c>
+      <c r="E4">
+        <v>54.79</v>
+      </c>
+      <c r="F4">
+        <v>53.42</v>
+      </c>
+      <c r="G4">
+        <v>52.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="8"/>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5">
+        <v>55.32</v>
+      </c>
+      <c r="D5">
+        <v>60.79</v>
+      </c>
+      <c r="E5">
+        <v>65.760000000000005</v>
+      </c>
+      <c r="F5">
+        <v>71.44</v>
+      </c>
+      <c r="G5">
+        <v>76.19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="8"/>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>55.64</v>
+      </c>
+      <c r="D6">
+        <v>60.63</v>
+      </c>
+      <c r="E6">
+        <v>65.209999999999994</v>
+      </c>
+      <c r="F6">
+        <v>70.540000000000006</v>
+      </c>
+      <c r="G6">
+        <v>74.98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E8">
+        <v>0.6</v>
+      </c>
+      <c r="F8">
+        <v>0.65</v>
+      </c>
+      <c r="G8">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="9"/>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>0.58904109589041098</v>
+      </c>
+      <c r="D9">
+        <v>0.54794520547945202</v>
+      </c>
+      <c r="E9">
+        <v>0.52054794520547898</v>
+      </c>
+      <c r="F9">
+        <v>0.50684931506849296</v>
+      </c>
+      <c r="G9">
+        <v>0.49315068493150699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="9"/>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10">
+        <v>0.44172661870503599</v>
+      </c>
+      <c r="D10">
+        <v>0.47338129496402898</v>
+      </c>
+      <c r="E10">
+        <v>0.50503597122302202</v>
+      </c>
+      <c r="F10">
+        <v>0.53237410071942404</v>
+      </c>
+      <c r="G10">
+        <v>0.55899280575539601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="9"/>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11">
+        <v>0.44907723855092302</v>
+      </c>
+      <c r="D11">
+        <v>0.47710184552289803</v>
+      </c>
+      <c r="E11">
+        <v>0.50580997949419004</v>
+      </c>
+      <c r="F11">
+        <v>0.53110047846889996</v>
+      </c>
+      <c r="G11">
+        <v>0.55570745044429304</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E13">
+        <v>0.6</v>
+      </c>
+      <c r="F13">
+        <v>0.65</v>
+      </c>
+      <c r="G13">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="9"/>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>0.69863013698630105</v>
+      </c>
+      <c r="D14">
+        <v>0.64383561643835596</v>
+      </c>
+      <c r="E14">
+        <v>0.57534246575342496</v>
+      </c>
+      <c r="F14">
+        <v>0.52054794520547898</v>
+      </c>
+      <c r="G14">
+        <v>0.465753424657534</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="9"/>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <v>0.492086330935252</v>
+      </c>
+      <c r="D15">
+        <v>0.536690647482014</v>
+      </c>
+      <c r="E15">
+        <v>0.57985611510791402</v>
+      </c>
+      <c r="F15">
+        <v>0.62158273381295004</v>
+      </c>
+      <c r="G15">
+        <v>0.66330935251798595</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="9"/>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16">
+        <v>0.50239234449760795</v>
+      </c>
+      <c r="D16">
+        <v>0.54203691045796298</v>
+      </c>
+      <c r="E16">
+        <v>0.57963089542036905</v>
+      </c>
+      <c r="F16">
+        <v>0.61654135338345895</v>
+      </c>
+      <c r="G16">
+        <v>0.65345181134654795</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A13:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" s="11" customFormat="1">
+      <c r="A2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>5.5</v>
+      </c>
+      <c r="C3">
+        <v>1.7</v>
+      </c>
+      <c r="D3">
+        <v>2.1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="F3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C4">
+        <v>2.7</v>
+      </c>
+      <c r="D4">
+        <v>1.6</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F4">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>3.4</v>
+      </c>
+      <c r="C5">
+        <v>2.9</v>
+      </c>
+      <c r="D5">
+        <v>1.9</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F5">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6">
+        <v>2.1</v>
+      </c>
+      <c r="C6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D6">
+        <v>1.6</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="F6">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>